<commit_message>
fill in form and download
</commit_message>
<xml_diff>
--- a/core/static/tenx/gsc_tenx_submission.xlsx
+++ b/core/static/tenx/gsc_tenx_submission.xlsx
@@ -1938,9 +1938,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="173" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="60" x14ac:knownFonts="1">
+  <fonts count="54" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2024,11 +2024,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
@@ -2041,26 +2036,8 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
@@ -2084,12 +2061,6 @@
       <b/>
       <sz val="10"/>
       <color indexed="62"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="10"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -2132,12 +2103,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color indexed="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color indexed="10"/>
@@ -2155,13 +2120,6 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color indexed="10"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -2337,6 +2295,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
     </font>
   </fonts>
   <fills count="12">
@@ -2658,7 +2621,7 @@
   </borders>
   <cellStyleXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -2777,109 +2740,106 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="173" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="173" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="173" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="173" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="173" fontId="41" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="173" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="40" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="3" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="3" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="3" borderId="3" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="3" borderId="3" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="43" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="43" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="36" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="36" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="43" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="36" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="3" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="3" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2887,189 +2847,190 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="49" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="56" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="49" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="46" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="49" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="42" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="49" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="10" borderId="4" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="10" borderId="4" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="5" borderId="18" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="5" borderId="18" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="18" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="5" borderId="18" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="58" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="58" fillId="6" borderId="18" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="6" borderId="18" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="18" xfId="28" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="5" borderId="18" xfId="28" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="3" xfId="20" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="3" xfId="20" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="43" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="43" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="71">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3489,8 +3450,8 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>165100</xdr:colOff>
-          <xdr:row>26</xdr:row>
-          <xdr:rowOff>190500</xdr:rowOff>
+          <xdr:row>27</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
@@ -3550,8 +3511,8 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>165100</xdr:colOff>
-          <xdr:row>27</xdr:row>
-          <xdr:rowOff>177800</xdr:rowOff>
+          <xdr:row>28</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
@@ -3611,14 +3572,14 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>812800</xdr:colOff>
-          <xdr:row>26</xdr:row>
-          <xdr:rowOff>203200</xdr:rowOff>
+          <xdr:row>27</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>1270000</xdr:colOff>
           <xdr:row>28</xdr:row>
-          <xdr:rowOff>25400</xdr:rowOff>
+          <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3672,14 +3633,14 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>812800</xdr:colOff>
-          <xdr:row>27</xdr:row>
-          <xdr:rowOff>190500</xdr:rowOff>
+          <xdr:row>28</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>1270000</xdr:colOff>
           <xdr:row>29</xdr:row>
-          <xdr:rowOff>25400</xdr:rowOff>
+          <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3733,14 +3694,14 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>812800</xdr:colOff>
-          <xdr:row>28</xdr:row>
-          <xdr:rowOff>190500</xdr:rowOff>
+          <xdr:row>29</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>1270000</xdr:colOff>
           <xdr:row>30</xdr:row>
-          <xdr:rowOff>25400</xdr:rowOff>
+          <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3794,8 +3755,8 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>165100</xdr:colOff>
-          <xdr:row>28</xdr:row>
-          <xdr:rowOff>177800</xdr:rowOff>
+          <xdr:row>29</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
@@ -4099,8 +4060,8 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>812800</xdr:colOff>
-          <xdr:row>29</xdr:row>
-          <xdr:rowOff>190500</xdr:rowOff>
+          <xdr:row>30</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
@@ -4160,8 +4121,8 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>165100</xdr:colOff>
-          <xdr:row>29</xdr:row>
-          <xdr:rowOff>177800</xdr:rowOff>
+          <xdr:row>30</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
@@ -4677,8 +4638,8 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:BX1433"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -4739,15 +4700,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:56" ht="19" thickTop="1">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="69" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
       <c r="E1" s="22"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="72"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="71"/>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
       <c r="J1" s="14"/>
@@ -4799,7 +4760,7 @@
       <c r="BD1" s="14"/>
     </row>
     <row r="2" spans="1:56">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="146" t="s">
         <v>132</v>
       </c>
       <c r="B2" s="23"/>
@@ -4807,7 +4768,7 @@
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
       <c r="F2" s="20"/>
-      <c r="G2" s="73"/>
+      <c r="G2" s="72"/>
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
       <c r="J2" s="14"/>
@@ -4867,7 +4828,7 @@
       <c r="D3" s="23"/>
       <c r="E3" s="23"/>
       <c r="F3" s="20"/>
-      <c r="G3" s="73"/>
+      <c r="G3" s="72"/>
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
       <c r="J3" s="14"/>
@@ -4927,7 +4888,7 @@
       <c r="D4" s="23"/>
       <c r="E4" s="23"/>
       <c r="F4" s="20"/>
-      <c r="G4" s="73"/>
+      <c r="G4" s="72"/>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
       <c r="J4" s="14"/>
@@ -4987,7 +4948,7 @@
       <c r="D5" s="23"/>
       <c r="E5" s="23"/>
       <c r="F5" s="20"/>
-      <c r="G5" s="73"/>
+      <c r="G5" s="72"/>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
       <c r="J5" s="14"/>
@@ -5047,7 +5008,7 @@
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
       <c r="F6" s="20"/>
-      <c r="G6" s="73"/>
+      <c r="G6" s="72"/>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
@@ -5107,7 +5068,7 @@
       <c r="D7" s="23"/>
       <c r="E7" s="23"/>
       <c r="F7" s="20"/>
-      <c r="G7" s="73"/>
+      <c r="G7" s="72"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
@@ -5167,7 +5128,7 @@
       <c r="D8" s="23"/>
       <c r="E8" s="23"/>
       <c r="F8" s="20"/>
-      <c r="G8" s="73"/>
+      <c r="G8" s="72"/>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
@@ -5219,13 +5180,13 @@
       <c r="BD8" s="14"/>
     </row>
     <row r="9" spans="1:56">
-      <c r="A9" s="74"/>
+      <c r="A9" s="73"/>
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
       <c r="E9" s="23"/>
       <c r="F9" s="20"/>
-      <c r="G9" s="73"/>
+      <c r="G9" s="72"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
@@ -5285,7 +5246,7 @@
       <c r="D10" s="23"/>
       <c r="E10" s="23"/>
       <c r="F10" s="20"/>
-      <c r="G10" s="73"/>
+      <c r="G10" s="72"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
@@ -5345,7 +5306,7 @@
       <c r="D11" s="23"/>
       <c r="E11" s="23"/>
       <c r="F11" s="20"/>
-      <c r="G11" s="73"/>
+      <c r="G11" s="72"/>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
@@ -5403,7 +5364,7 @@
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
       <c r="F12" s="20"/>
-      <c r="G12" s="73"/>
+      <c r="G12" s="72"/>
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
@@ -5455,13 +5416,13 @@
       <c r="BD12" s="14"/>
     </row>
     <row r="13" spans="1:56" ht="13" thickBot="1">
-      <c r="A13" s="75"/>
-      <c r="B13" s="76"/>
-      <c r="C13" s="76"/>
-      <c r="D13" s="76"/>
-      <c r="E13" s="76"/>
-      <c r="F13" s="76"/>
-      <c r="G13" s="77"/>
+      <c r="A13" s="74"/>
+      <c r="B13" s="75"/>
+      <c r="C13" s="75"/>
+      <c r="D13" s="75"/>
+      <c r="E13" s="75"/>
+      <c r="F13" s="75"/>
+      <c r="G13" s="76"/>
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
       <c r="J13" s="14"/>
@@ -5635,7 +5596,7 @@
       <c r="J16" s="9"/>
     </row>
     <row r="17" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A17" s="78" t="s">
+      <c r="A17" s="77" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="41" t="s">
@@ -5651,7 +5612,7 @@
       <c r="J17" s="9"/>
     </row>
     <row r="18" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A18" s="79" t="s">
+      <c r="A18" s="78" t="s">
         <v>81</v>
       </c>
       <c r="B18" s="38" t="s">
@@ -5667,10 +5628,10 @@
       <c r="J18" s="9"/>
     </row>
     <row r="19" spans="1:10" s="3" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A19" s="78" t="s">
+      <c r="A19" s="77" t="s">
         <v>82</v>
       </c>
-      <c r="B19" s="121" t="s">
+      <c r="B19" s="120" t="s">
         <v>181</v>
       </c>
       <c r="C19" s="18"/>
@@ -5683,7 +5644,7 @@
       <c r="J19" s="9"/>
     </row>
     <row r="20" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A20" s="78" t="s">
+      <c r="A20" s="77" t="s">
         <v>2</v>
       </c>
       <c r="B20" s="39"/>
@@ -5697,10 +5658,10 @@
       <c r="J20" s="9"/>
     </row>
     <row r="21" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A21" s="78" t="s">
+      <c r="A21" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="121"/>
+      <c r="B21" s="120"/>
       <c r="C21" s="18"/>
       <c r="D21" s="18"/>
       <c r="E21" s="18"/>
@@ -5711,7 +5672,7 @@
       <c r="J21" s="9"/>
     </row>
     <row r="22" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A22" s="78" t="s">
+      <c r="A22" s="77" t="s">
         <v>0</v>
       </c>
       <c r="B22" s="39"/>
@@ -5724,7 +5685,7 @@
       <c r="J22" s="9"/>
     </row>
     <row r="23" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A23" s="78" t="s">
+      <c r="A23" s="77" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="38" t="s">
@@ -5740,7 +5701,7 @@
       <c r="J23" s="9"/>
     </row>
     <row r="24" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A24" s="80" t="s">
+      <c r="A24" s="79" t="s">
         <v>12</v>
       </c>
       <c r="B24" s="40" t="s">
@@ -5780,7 +5741,7 @@
       <c r="J26" s="9"/>
     </row>
     <row r="27" spans="1:10" ht="15" thickBot="1">
-      <c r="A27" s="85" t="s">
+      <c r="A27" s="84" t="s">
         <v>148</v>
       </c>
       <c r="C27" s="19"/>
@@ -5790,7 +5751,7 @@
       <c r="J27" s="9"/>
     </row>
     <row r="28" spans="1:10" ht="14">
-      <c r="A28" s="82" t="s">
+      <c r="A28" s="81" t="s">
         <v>93</v>
       </c>
       <c r="C28" s="19"/>
@@ -5800,7 +5761,7 @@
       <c r="J28" s="9"/>
     </row>
     <row r="29" spans="1:10" ht="14">
-      <c r="A29" s="83" t="s">
+      <c r="A29" s="82" t="s">
         <v>127</v>
       </c>
       <c r="C29" s="19"/>
@@ -5810,7 +5771,7 @@
       <c r="J29" s="9"/>
     </row>
     <row r="30" spans="1:10" ht="14">
-      <c r="A30" s="83" t="s">
+      <c r="A30" s="82" t="s">
         <v>156</v>
       </c>
       <c r="C30" s="19"/>
@@ -5820,7 +5781,7 @@
       <c r="J30" s="9"/>
     </row>
     <row r="31" spans="1:10" ht="15">
-      <c r="A31" s="83" t="s">
+      <c r="A31" s="82" t="s">
         <v>104</v>
       </c>
       <c r="C31" s="36"/>
@@ -5830,8 +5791,8 @@
       <c r="J31" s="9"/>
     </row>
     <row r="32" spans="1:10" ht="16" thickBot="1">
-      <c r="A32" s="80"/>
-      <c r="B32" s="81"/>
+      <c r="A32" s="79"/>
+      <c r="B32" s="80"/>
       <c r="C32" s="36"/>
       <c r="G32" s="9"/>
       <c r="H32" s="9"/>
@@ -5839,10 +5800,10 @@
       <c r="J32" s="9"/>
     </row>
     <row r="33" spans="1:10" ht="16" thickBot="1">
-      <c r="A33" s="84" t="s">
+      <c r="A33" s="83" t="s">
         <v>134</v>
       </c>
-      <c r="B33" s="81"/>
+      <c r="B33" s="80"/>
       <c r="C33" s="36"/>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
@@ -5850,8 +5811,8 @@
       <c r="J33" s="9"/>
     </row>
     <row r="34" spans="1:10" ht="16" thickBot="1">
-      <c r="A34" s="80"/>
-      <c r="B34" s="81"/>
+      <c r="A34" s="79"/>
+      <c r="B34" s="80"/>
       <c r="C34" s="36"/>
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
@@ -5859,11 +5820,11 @@
       <c r="J34" s="9"/>
     </row>
     <row r="35" spans="1:10" ht="14">
-      <c r="A35" s="97" t="s">
+      <c r="A35" s="96" t="s">
         <v>147</v>
       </c>
-      <c r="B35" s="81"/>
-      <c r="C35" s="100" t="s">
+      <c r="B35" s="80"/>
+      <c r="C35" s="99" t="s">
         <v>177</v>
       </c>
       <c r="G35" s="9"/>
@@ -5872,10 +5833,10 @@
       <c r="J35" s="9"/>
     </row>
     <row r="36" spans="1:10" ht="14">
-      <c r="A36" s="98" t="s">
+      <c r="A36" s="97" t="s">
         <v>160</v>
       </c>
-      <c r="B36" s="100" t="s">
+      <c r="B36" s="99" t="s">
         <v>154</v>
       </c>
       <c r="C36" s="19"/>
@@ -5885,10 +5846,10 @@
       <c r="J36" s="9"/>
     </row>
     <row r="37" spans="1:10" ht="14">
-      <c r="A37" s="99" t="s">
+      <c r="A37" s="98" t="s">
         <v>161</v>
       </c>
-      <c r="B37" s="96" t="s">
+      <c r="B37" s="95" t="s">
         <v>151</v>
       </c>
       <c r="C37" s="19"/>
@@ -5898,10 +5859,10 @@
       <c r="J37" s="9"/>
     </row>
     <row r="38" spans="1:10" ht="14">
-      <c r="A38" s="99" t="s">
+      <c r="A38" s="98" t="s">
         <v>152</v>
       </c>
-      <c r="B38" s="90" t="s">
+      <c r="B38" s="89" t="s">
         <v>153</v>
       </c>
       <c r="C38" s="19"/>
@@ -5911,7 +5872,7 @@
       <c r="J38" s="9"/>
     </row>
     <row r="39" spans="1:10" ht="15" thickBot="1">
-      <c r="A39" s="80"/>
+      <c r="A39" s="79"/>
       <c r="B39" s="45"/>
       <c r="C39" s="19"/>
       <c r="G39" s="9"/>
@@ -5920,7 +5881,7 @@
       <c r="J39" s="9"/>
     </row>
     <row r="40" spans="1:10" ht="15" thickBot="1">
-      <c r="A40" s="86" t="s">
+      <c r="A40" s="85" t="s">
         <v>135</v>
       </c>
       <c r="G40" s="9"/>
@@ -5929,7 +5890,7 @@
       <c r="J40" s="9"/>
     </row>
     <row r="41" spans="1:10" ht="14">
-      <c r="A41" s="87" t="s">
+      <c r="A41" s="86" t="s">
         <v>95</v>
       </c>
       <c r="G41" s="9"/>
@@ -5938,37 +5899,37 @@
       <c r="J41" s="9"/>
     </row>
     <row r="42" spans="1:10" ht="14">
-      <c r="A42" s="88" t="s">
+      <c r="A42" s="87" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="14">
-      <c r="A43" s="88" t="s">
+      <c r="A43" s="87" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="14">
-      <c r="A44" s="88" t="s">
+      <c r="A44" s="87" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="14">
-      <c r="A45" s="88" t="s">
+      <c r="A45" s="87" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="14">
-      <c r="A46" s="88" t="s">
+      <c r="A46" s="87" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="14">
-      <c r="A47" s="88" t="s">
+      <c r="A47" s="87" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="14">
-      <c r="A48" s="88" t="s">
+      <c r="A48" s="87" t="s">
         <v>102</v>
       </c>
     </row>
@@ -5977,7 +5938,7 @@
       <c r="B49" s="17"/>
     </row>
     <row r="50" spans="1:68" ht="15">
-      <c r="A50" s="80" t="s">
+      <c r="A50" s="79" t="s">
         <v>70</v>
       </c>
       <c r="B50" s="17"/>
@@ -5987,7 +5948,7 @@
       </c>
     </row>
     <row r="51" spans="1:68" ht="18" customHeight="1">
-      <c r="A51" s="80"/>
+      <c r="A51" s="79"/>
       <c r="B51" s="17"/>
       <c r="C51" s="37" t="str">
         <f>IF('Checkbox Status'!A3=TRUE, "GSC will destroy any remaining sample at completion of project","")</f>
@@ -5995,29 +5956,29 @@
       </c>
     </row>
     <row r="52" spans="1:68" ht="15">
-      <c r="A52" s="80"/>
+      <c r="A52" s="79"/>
       <c r="B52" s="45"/>
       <c r="C52" s="37"/>
     </row>
     <row r="53" spans="1:68" ht="15">
-      <c r="A53" s="80" t="s">
+      <c r="A53" s="79" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="90" t="s">
+      <c r="B53" s="89" t="s">
         <v>83</v>
       </c>
       <c r="C53" s="37"/>
     </row>
     <row r="54" spans="1:68" ht="15">
-      <c r="A54" s="80"/>
+      <c r="A54" s="79"/>
       <c r="B54" s="45"/>
       <c r="C54" s="37"/>
     </row>
     <row r="55" spans="1:68" ht="14">
-      <c r="A55" s="89" t="s">
+      <c r="A55" s="88" t="s">
         <v>136</v>
       </c>
-      <c r="B55" s="90" t="s">
+      <c r="B55" s="89" t="s">
         <v>4</v>
       </c>
       <c r="C55" s="10"/>
@@ -6027,74 +5988,74 @@
     </row>
     <row r="56" spans="1:68" ht="14">
       <c r="A56" s="45"/>
-      <c r="B56" s="90"/>
-      <c r="C56" s="91"/>
-      <c r="D56" s="91"/>
-      <c r="E56" s="91"/>
-      <c r="F56" s="91"/>
+      <c r="B56" s="89"/>
+      <c r="C56" s="90"/>
+      <c r="D56" s="90"/>
+      <c r="E56" s="90"/>
+      <c r="F56" s="90"/>
       <c r="G56" s="45"/>
       <c r="H56" s="45"/>
       <c r="I56" s="45"/>
     </row>
     <row r="57" spans="1:68" ht="14">
-      <c r="A57" s="92" t="s">
+      <c r="A57" s="91" t="s">
         <v>160</v>
       </c>
-      <c r="B57" s="93" t="s">
+      <c r="B57" s="92" t="s">
         <v>91</v>
       </c>
-      <c r="C57" s="91"/>
-      <c r="D57" s="91"/>
-      <c r="E57" s="91"/>
-      <c r="F57" s="91"/>
+      <c r="C57" s="90"/>
+      <c r="D57" s="90"/>
+      <c r="E57" s="90"/>
+      <c r="F57" s="90"/>
       <c r="G57" s="45"/>
       <c r="H57" s="45"/>
       <c r="I57" s="45"/>
     </row>
     <row r="58" spans="1:68" ht="14">
-      <c r="A58" s="94"/>
-      <c r="B58" s="93" t="s">
+      <c r="A58" s="93"/>
+      <c r="B58" s="92" t="s">
         <v>92</v>
       </c>
-      <c r="C58" s="91"/>
-      <c r="D58" s="91"/>
-      <c r="E58" s="91"/>
-      <c r="F58" s="91"/>
+      <c r="C58" s="90"/>
+      <c r="D58" s="90"/>
+      <c r="E58" s="90"/>
+      <c r="F58" s="90"/>
       <c r="G58" s="45"/>
       <c r="H58" s="45"/>
       <c r="I58" s="45"/>
     </row>
     <row r="59" spans="1:68" ht="14">
       <c r="A59" s="45"/>
-      <c r="B59" s="93"/>
-      <c r="C59" s="91"/>
-      <c r="D59" s="91"/>
-      <c r="E59" s="91"/>
-      <c r="F59" s="91"/>
+      <c r="B59" s="92"/>
+      <c r="C59" s="90"/>
+      <c r="D59" s="90"/>
+      <c r="E59" s="90"/>
+      <c r="F59" s="90"/>
       <c r="G59" s="45"/>
       <c r="H59" s="45"/>
       <c r="I59" s="45"/>
     </row>
     <row r="60" spans="1:68" ht="14">
-      <c r="A60" s="101" t="s">
+      <c r="A60" s="100" t="s">
         <v>149</v>
       </c>
-      <c r="B60" s="93"/>
-      <c r="C60" s="91"/>
-      <c r="D60" s="91"/>
-      <c r="E60" s="91"/>
-      <c r="F60" s="91"/>
+      <c r="B60" s="92"/>
+      <c r="C60" s="90"/>
+      <c r="D60" s="90"/>
+      <c r="E60" s="90"/>
+      <c r="F60" s="90"/>
       <c r="G60" s="45"/>
       <c r="H60" s="45"/>
       <c r="I60" s="45"/>
     </row>
     <row r="61" spans="1:68" ht="14">
-      <c r="A61" s="95"/>
-      <c r="B61" s="93"/>
-      <c r="C61" s="91"/>
-      <c r="D61" s="91"/>
-      <c r="E61" s="91"/>
-      <c r="F61" s="91"/>
+      <c r="A61" s="94"/>
+      <c r="B61" s="92"/>
+      <c r="C61" s="90"/>
+      <c r="D61" s="90"/>
+      <c r="E61" s="90"/>
+      <c r="F61" s="90"/>
       <c r="G61" s="45"/>
       <c r="H61" s="45"/>
       <c r="I61" s="45"/>
@@ -6183,14 +6144,14 @@
       <c r="E63" s="135"/>
       <c r="F63" s="135"/>
       <c r="G63" s="136"/>
-      <c r="H63" s="128" t="s">
+      <c r="H63" s="130" t="s">
         <v>50</v>
       </c>
-      <c r="I63" s="129"/>
-      <c r="J63" s="129"/>
-      <c r="K63" s="129"/>
-      <c r="L63" s="129"/>
-      <c r="M63" s="130"/>
+      <c r="I63" s="131"/>
+      <c r="J63" s="131"/>
+      <c r="K63" s="131"/>
+      <c r="L63" s="131"/>
+      <c r="M63" s="132"/>
       <c r="N63" s="134" t="s">
         <v>11</v>
       </c>
@@ -6241,124 +6202,124 @@
       <c r="BF63" s="53"/>
       <c r="BG63" s="53"/>
     </row>
-    <row r="64" spans="1:68" s="106" customFormat="1" ht="84">
-      <c r="A64" s="102" t="s">
+    <row r="64" spans="1:68" s="105" customFormat="1" ht="84">
+      <c r="A64" s="101" t="s">
         <v>162</v>
       </c>
-      <c r="B64" s="102" t="s">
+      <c r="B64" s="101" t="s">
         <v>117</v>
       </c>
-      <c r="C64" s="103" t="s">
+      <c r="C64" s="102" t="s">
         <v>118</v>
       </c>
-      <c r="D64" s="104" t="s">
+      <c r="D64" s="103" t="s">
         <v>56</v>
       </c>
-      <c r="E64" s="104" t="s">
+      <c r="E64" s="103" t="s">
         <v>85</v>
       </c>
-      <c r="F64" s="104" t="s">
+      <c r="F64" s="103" t="s">
         <v>119</v>
       </c>
-      <c r="G64" s="104" t="s">
+      <c r="G64" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="H64" s="102" t="s">
+      <c r="H64" s="101" t="s">
         <v>120</v>
       </c>
-      <c r="I64" s="102" t="s">
+      <c r="I64" s="101" t="s">
         <v>176</v>
       </c>
-      <c r="J64" s="102" t="s">
+      <c r="J64" s="101" t="s">
         <v>175</v>
       </c>
-      <c r="K64" s="102" t="s">
+      <c r="K64" s="101" t="s">
         <v>48</v>
       </c>
-      <c r="L64" s="102" t="s">
+      <c r="L64" s="101" t="s">
         <v>86</v>
       </c>
-      <c r="M64" s="102" t="s">
+      <c r="M64" s="101" t="s">
         <v>121</v>
       </c>
-      <c r="N64" s="104" t="s">
+      <c r="N64" s="103" t="s">
         <v>140</v>
       </c>
-      <c r="O64" s="104" t="s">
+      <c r="O64" s="103" t="s">
         <v>141</v>
       </c>
-      <c r="P64" s="104" t="s">
+      <c r="P64" s="103" t="s">
         <v>142</v>
       </c>
-      <c r="Q64" s="104" t="s">
+      <c r="Q64" s="103" t="s">
         <v>143</v>
       </c>
-      <c r="R64" s="104" t="s">
+      <c r="R64" s="103" t="s">
         <v>138</v>
       </c>
-      <c r="S64" s="104" t="s">
+      <c r="S64" s="103" t="s">
         <v>139</v>
       </c>
       <c r="T64" s="138"/>
-      <c r="U64" s="105"/>
-      <c r="W64" s="105"/>
-      <c r="X64" s="105"/>
-      <c r="Y64" s="105"/>
-      <c r="Z64" s="105"/>
-      <c r="AA64" s="105"/>
-      <c r="AB64" s="105"/>
-      <c r="AC64" s="105"/>
-      <c r="AD64" s="105"/>
-      <c r="AE64" s="105"/>
-      <c r="AF64" s="105"/>
-      <c r="AG64" s="105"/>
-      <c r="AH64" s="105"/>
-      <c r="AI64" s="105"/>
-      <c r="AJ64" s="105"/>
-      <c r="AK64" s="105"/>
-      <c r="AL64" s="105"/>
-      <c r="AM64" s="105"/>
-      <c r="AN64" s="105"/>
-      <c r="AO64" s="105"/>
-      <c r="AP64" s="105"/>
-      <c r="AQ64" s="105"/>
-      <c r="AR64" s="105"/>
-      <c r="AS64" s="105"/>
-      <c r="AT64" s="105"/>
-      <c r="AU64" s="105"/>
-      <c r="AV64" s="105"/>
-      <c r="AW64" s="105"/>
-      <c r="AX64" s="105"/>
-      <c r="AY64" s="105"/>
-      <c r="AZ64" s="105"/>
-      <c r="BA64" s="105"/>
-      <c r="BB64" s="105"/>
-      <c r="BC64" s="105"/>
-      <c r="BD64" s="105"/>
-      <c r="BE64" s="105"/>
-      <c r="BF64" s="105"/>
-      <c r="BG64" s="105"/>
+      <c r="U64" s="104"/>
+      <c r="W64" s="104"/>
+      <c r="X64" s="104"/>
+      <c r="Y64" s="104"/>
+      <c r="Z64" s="104"/>
+      <c r="AA64" s="104"/>
+      <c r="AB64" s="104"/>
+      <c r="AC64" s="104"/>
+      <c r="AD64" s="104"/>
+      <c r="AE64" s="104"/>
+      <c r="AF64" s="104"/>
+      <c r="AG64" s="104"/>
+      <c r="AH64" s="104"/>
+      <c r="AI64" s="104"/>
+      <c r="AJ64" s="104"/>
+      <c r="AK64" s="104"/>
+      <c r="AL64" s="104"/>
+      <c r="AM64" s="104"/>
+      <c r="AN64" s="104"/>
+      <c r="AO64" s="104"/>
+      <c r="AP64" s="104"/>
+      <c r="AQ64" s="104"/>
+      <c r="AR64" s="104"/>
+      <c r="AS64" s="104"/>
+      <c r="AT64" s="104"/>
+      <c r="AU64" s="104"/>
+      <c r="AV64" s="104"/>
+      <c r="AW64" s="104"/>
+      <c r="AX64" s="104"/>
+      <c r="AY64" s="104"/>
+      <c r="AZ64" s="104"/>
+      <c r="BA64" s="104"/>
+      <c r="BB64" s="104"/>
+      <c r="BC64" s="104"/>
+      <c r="BD64" s="104"/>
+      <c r="BE64" s="104"/>
+      <c r="BF64" s="104"/>
+      <c r="BG64" s="104"/>
     </row>
     <row r="65" spans="1:69" s="65" customFormat="1" ht="15" thickBot="1">
-      <c r="A65" s="119" t="s">
+      <c r="A65" s="118" t="s">
         <v>74</v>
       </c>
-      <c r="B65" s="119" t="s">
+      <c r="B65" s="118" t="s">
         <v>74</v>
       </c>
-      <c r="C65" s="119" t="s">
+      <c r="C65" s="118" t="s">
         <v>74</v>
       </c>
-      <c r="D65" s="120" t="s">
+      <c r="D65" s="119" t="s">
         <v>74</v>
       </c>
       <c r="E65" s="66" t="s">
         <v>74</v>
       </c>
-      <c r="F65" s="120" t="s">
+      <c r="F65" s="119" t="s">
         <v>74</v>
       </c>
-      <c r="G65" s="120" t="s">
+      <c r="G65" s="119" t="s">
         <v>74</v>
       </c>
       <c r="H65" s="66" t="s">
@@ -6379,16 +6340,16 @@
       <c r="M65" s="66" t="s">
         <v>74</v>
       </c>
-      <c r="N65" s="120" t="s">
+      <c r="N65" s="119" t="s">
         <v>74</v>
       </c>
-      <c r="O65" s="120" t="s">
+      <c r="O65" s="119" t="s">
         <v>74</v>
       </c>
-      <c r="P65" s="120" t="s">
+      <c r="P65" s="119" t="s">
         <v>74</v>
       </c>
-      <c r="Q65" s="120" t="s">
+      <c r="Q65" s="119" t="s">
         <v>74</v>
       </c>
       <c r="R65" s="66" t="s">
@@ -6397,7 +6358,7 @@
       <c r="S65" s="66" t="s">
         <v>74</v>
       </c>
-      <c r="T65" s="120" t="s">
+      <c r="T65" s="119" t="s">
         <v>74</v>
       </c>
       <c r="U65" s="64"/>
@@ -6440,13 +6401,13 @@
       <c r="BG65" s="64"/>
     </row>
     <row r="66" spans="1:69" s="68" customFormat="1" ht="16" thickTop="1">
-      <c r="A66" s="126"/>
-      <c r="B66" s="126"/>
-      <c r="C66" s="124">
+      <c r="A66" s="125"/>
+      <c r="B66" s="125"/>
+      <c r="C66" s="123">
         <v>9606</v>
       </c>
-      <c r="D66" s="124"/>
-      <c r="E66" s="124">
+      <c r="D66" s="123"/>
+      <c r="E66" s="123">
         <v>4</v>
       </c>
       <c r="F66" s="62" t="s">
@@ -6468,7 +6429,7 @@
       <c r="L66" s="62">
         <v>469</v>
       </c>
-      <c r="M66" s="125">
+      <c r="M66" s="124">
         <v>4</v>
       </c>
       <c r="N66" s="62" t="s">
@@ -6486,7 +6447,7 @@
       <c r="R66" s="62" t="s">
         <v>123</v>
       </c>
-      <c r="T66" s="122"/>
+      <c r="T66" s="121"/>
       <c r="U66" s="62"/>
       <c r="V66" s="62"/>
       <c r="W66" s="62"/>
@@ -6942,32 +6903,32 @@
       <c r="BP72" s="31"/>
     </row>
     <row r="73" spans="1:69" s="54" customFormat="1" ht="24" customHeight="1">
-      <c r="A73" s="131" t="s">
+      <c r="A73" s="133" t="s">
         <v>155</v>
       </c>
-      <c r="B73" s="132"/>
-      <c r="C73" s="132"/>
-      <c r="D73" s="132"/>
-      <c r="E73" s="132"/>
-      <c r="F73" s="132"/>
-      <c r="G73" s="132"/>
-      <c r="H73" s="133"/>
-      <c r="I73" s="146" t="s">
+      <c r="B73" s="128"/>
+      <c r="C73" s="128"/>
+      <c r="D73" s="128"/>
+      <c r="E73" s="128"/>
+      <c r="F73" s="128"/>
+      <c r="G73" s="128"/>
+      <c r="H73" s="129"/>
+      <c r="I73" s="127" t="s">
         <v>8</v>
       </c>
-      <c r="J73" s="132"/>
-      <c r="K73" s="132"/>
-      <c r="L73" s="132"/>
-      <c r="M73" s="132"/>
-      <c r="N73" s="133"/>
-      <c r="O73" s="131" t="s">
+      <c r="J73" s="128"/>
+      <c r="K73" s="128"/>
+      <c r="L73" s="128"/>
+      <c r="M73" s="128"/>
+      <c r="N73" s="129"/>
+      <c r="O73" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="P73" s="132"/>
-      <c r="Q73" s="132"/>
-      <c r="R73" s="132"/>
-      <c r="S73" s="132"/>
-      <c r="T73" s="133"/>
+      <c r="P73" s="128"/>
+      <c r="Q73" s="128"/>
+      <c r="R73" s="128"/>
+      <c r="S73" s="128"/>
+      <c r="T73" s="129"/>
       <c r="U73" s="63" t="s">
         <v>58</v>
       </c>
@@ -6977,10 +6938,10 @@
       <c r="W73" s="140" t="s">
         <v>126</v>
       </c>
-      <c r="X73" s="132"/>
-      <c r="Y73" s="132"/>
-      <c r="Z73" s="133"/>
-      <c r="AA73" s="131" t="s">
+      <c r="X73" s="128"/>
+      <c r="Y73" s="128"/>
+      <c r="Z73" s="129"/>
+      <c r="AA73" s="133" t="s">
         <v>50</v>
       </c>
       <c r="AB73" s="141"/>
@@ -7019,157 +6980,157 @@
       <c r="BG73" s="53"/>
       <c r="BH73" s="53"/>
     </row>
-    <row r="74" spans="1:69" s="118" customFormat="1" ht="84">
-      <c r="A74" s="107" t="s">
+    <row r="74" spans="1:69" s="117" customFormat="1" ht="84">
+      <c r="A74" s="106" t="s">
         <v>115</v>
       </c>
-      <c r="B74" s="107" t="s">
+      <c r="B74" s="106" t="s">
         <v>106</v>
       </c>
-      <c r="C74" s="108" t="s">
+      <c r="C74" s="107" t="s">
         <v>107</v>
       </c>
-      <c r="D74" s="109" t="s">
+      <c r="D74" s="108" t="s">
         <v>128</v>
       </c>
-      <c r="E74" s="109" t="s">
+      <c r="E74" s="108" t="s">
         <v>41</v>
       </c>
-      <c r="F74" s="109" t="s">
+      <c r="F74" s="108" t="s">
         <v>76</v>
       </c>
-      <c r="G74" s="110" t="s">
+      <c r="G74" s="109" t="s">
         <v>108</v>
       </c>
-      <c r="H74" s="109" t="s">
+      <c r="H74" s="108" t="s">
         <v>109</v>
       </c>
-      <c r="I74" s="111" t="s">
+      <c r="I74" s="110" t="s">
         <v>9</v>
       </c>
-      <c r="J74" s="112" t="s">
+      <c r="J74" s="111" t="s">
         <v>10</v>
       </c>
-      <c r="K74" s="113" t="s">
+      <c r="K74" s="112" t="s">
         <v>75</v>
       </c>
-      <c r="L74" s="111" t="s">
+      <c r="L74" s="110" t="s">
         <v>110</v>
       </c>
-      <c r="M74" s="112" t="s">
+      <c r="M74" s="111" t="s">
         <v>146</v>
       </c>
-      <c r="N74" s="112" t="s">
+      <c r="N74" s="111" t="s">
         <v>7</v>
       </c>
-      <c r="O74" s="107" t="s">
+      <c r="O74" s="106" t="s">
         <v>125</v>
       </c>
-      <c r="P74" s="114" t="s">
+      <c r="P74" s="113" t="s">
         <v>77</v>
       </c>
-      <c r="Q74" s="109" t="s">
+      <c r="Q74" s="108" t="s">
         <v>17</v>
       </c>
-      <c r="R74" s="109" t="s">
+      <c r="R74" s="108" t="s">
         <v>18</v>
       </c>
-      <c r="S74" s="109" t="s">
+      <c r="S74" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="T74" s="109" t="s">
+      <c r="T74" s="108" t="s">
         <v>112</v>
       </c>
-      <c r="U74" s="112" t="s">
+      <c r="U74" s="111" t="s">
         <v>111</v>
       </c>
-      <c r="V74" s="109" t="s">
+      <c r="V74" s="108" t="s">
         <v>78</v>
       </c>
-      <c r="W74" s="112" t="s">
+      <c r="W74" s="111" t="s">
         <v>56</v>
       </c>
-      <c r="X74" s="112" t="s">
+      <c r="X74" s="111" t="s">
         <v>85</v>
       </c>
-      <c r="Y74" s="112" t="s">
+      <c r="Y74" s="111" t="s">
         <v>113</v>
       </c>
-      <c r="Z74" s="112" t="s">
+      <c r="Z74" s="111" t="s">
         <v>57</v>
       </c>
-      <c r="AA74" s="109" t="s">
+      <c r="AA74" s="108" t="s">
         <v>114</v>
       </c>
-      <c r="AB74" s="109" t="s">
+      <c r="AB74" s="108" t="s">
         <v>178</v>
       </c>
-      <c r="AC74" s="109" t="s">
+      <c r="AC74" s="108" t="s">
         <v>48</v>
       </c>
-      <c r="AD74" s="109" t="s">
+      <c r="AD74" s="108" t="s">
         <v>86</v>
       </c>
-      <c r="AE74" s="107" t="s">
+      <c r="AE74" s="106" t="s">
         <v>150</v>
       </c>
-      <c r="AF74" s="107" t="s">
+      <c r="AF74" s="106" t="s">
         <v>116</v>
       </c>
-      <c r="AG74" s="107" t="s">
+      <c r="AG74" s="106" t="s">
         <v>157</v>
       </c>
-      <c r="AH74" s="115" t="s">
+      <c r="AH74" s="114" t="s">
         <v>51</v>
       </c>
-      <c r="AI74" s="115" t="s">
+      <c r="AI74" s="114" t="s">
         <v>42</v>
       </c>
-      <c r="AJ74" s="115" t="s">
+      <c r="AJ74" s="114" t="s">
         <v>43</v>
       </c>
-      <c r="AK74" s="115" t="s">
+      <c r="AK74" s="114" t="s">
         <v>44</v>
       </c>
-      <c r="AL74" s="115" t="s">
+      <c r="AL74" s="114" t="s">
         <v>45</v>
       </c>
-      <c r="AM74" s="115" t="s">
+      <c r="AM74" s="114" t="s">
         <v>46</v>
       </c>
-      <c r="AN74" s="115" t="s">
+      <c r="AN74" s="114" t="s">
         <v>165</v>
       </c>
-      <c r="AO74" s="115" t="s">
+      <c r="AO74" s="114" t="s">
         <v>47</v>
       </c>
-      <c r="AP74" s="115" t="s">
+      <c r="AP74" s="114" t="s">
         <v>166</v>
       </c>
-      <c r="AQ74" s="115" t="s">
+      <c r="AQ74" s="114" t="s">
         <v>167</v>
       </c>
-      <c r="AR74" s="115" t="s">
+      <c r="AR74" s="114" t="s">
         <v>168</v>
       </c>
-      <c r="AS74" s="115" t="s">
+      <c r="AS74" s="114" t="s">
         <v>169</v>
       </c>
-      <c r="AT74" s="116"/>
-      <c r="AU74" s="117"/>
-      <c r="AV74" s="117"/>
-      <c r="AW74" s="117"/>
-      <c r="AX74" s="117"/>
-      <c r="AY74" s="117"/>
-      <c r="AZ74" s="117"/>
-      <c r="BA74" s="117"/>
-      <c r="BB74" s="117"/>
-      <c r="BC74" s="117"/>
-      <c r="BD74" s="117"/>
-      <c r="BE74" s="117"/>
-      <c r="BF74" s="117"/>
-      <c r="BG74" s="117"/>
-      <c r="BH74" s="117"/>
+      <c r="AT74" s="115"/>
+      <c r="AU74" s="116"/>
+      <c r="AV74" s="116"/>
+      <c r="AW74" s="116"/>
+      <c r="AX74" s="116"/>
+      <c r="AY74" s="116"/>
+      <c r="AZ74" s="116"/>
+      <c r="BA74" s="116"/>
+      <c r="BB74" s="116"/>
+      <c r="BC74" s="116"/>
+      <c r="BD74" s="116"/>
+      <c r="BE74" s="116"/>
+      <c r="BF74" s="116"/>
+      <c r="BG74" s="116"/>
+      <c r="BH74" s="116"/>
     </row>
     <row r="75" spans="1:69" s="52" customFormat="1" ht="15" thickBot="1">
       <c r="A75" s="49" t="s">
@@ -7178,76 +7139,76 @@
       <c r="B75" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="C75" s="119" t="s">
+      <c r="C75" s="118" t="s">
         <v>74</v>
       </c>
-      <c r="D75" s="119" t="s">
+      <c r="D75" s="118" t="s">
         <v>74</v>
       </c>
-      <c r="E75" s="119" t="s">
+      <c r="E75" s="118" t="s">
         <v>74</v>
       </c>
-      <c r="F75" s="119" t="s">
+      <c r="F75" s="118" t="s">
         <v>74</v>
       </c>
-      <c r="G75" s="119" t="s">
+      <c r="G75" s="118" t="s">
         <v>74</v>
       </c>
-      <c r="H75" s="119" t="s">
+      <c r="H75" s="118" t="s">
         <v>74</v>
       </c>
-      <c r="I75" s="119" t="s">
+      <c r="I75" s="118" t="s">
         <v>74</v>
       </c>
-      <c r="J75" s="120" t="s">
+      <c r="J75" s="119" t="s">
         <v>74</v>
       </c>
-      <c r="K75" s="120" t="s">
+      <c r="K75" s="119" t="s">
         <v>74</v>
       </c>
-      <c r="L75" s="120" t="s">
+      <c r="L75" s="119" t="s">
         <v>74</v>
       </c>
-      <c r="M75" s="120" t="s">
+      <c r="M75" s="119" t="s">
         <v>74</v>
       </c>
-      <c r="N75" s="120" t="s">
+      <c r="N75" s="119" t="s">
         <v>74</v>
       </c>
-      <c r="O75" s="120" t="s">
+      <c r="O75" s="119" t="s">
         <v>74</v>
       </c>
-      <c r="P75" s="120" t="s">
+      <c r="P75" s="119" t="s">
         <v>74</v>
       </c>
-      <c r="Q75" s="120" t="s">
+      <c r="Q75" s="119" t="s">
         <v>74</v>
       </c>
-      <c r="R75" s="120" t="s">
+      <c r="R75" s="119" t="s">
         <v>74</v>
       </c>
-      <c r="S75" s="120" t="s">
+      <c r="S75" s="119" t="s">
         <v>74</v>
       </c>
-      <c r="T75" s="120" t="s">
+      <c r="T75" s="119" t="s">
         <v>74</v>
       </c>
-      <c r="U75" s="120" t="s">
+      <c r="U75" s="119" t="s">
         <v>74</v>
       </c>
-      <c r="V75" s="120" t="s">
+      <c r="V75" s="119" t="s">
         <v>74</v>
       </c>
-      <c r="W75" s="120" t="s">
+      <c r="W75" s="119" t="s">
         <v>74</v>
       </c>
       <c r="X75" s="66" t="s">
         <v>74</v>
       </c>
-      <c r="Y75" s="120" t="s">
+      <c r="Y75" s="119" t="s">
         <v>74</v>
       </c>
-      <c r="Z75" s="120" t="s">
+      <c r="Z75" s="119" t="s">
         <v>74</v>
       </c>
       <c r="AA75" s="66" t="s">
@@ -7280,22 +7241,22 @@
       <c r="AJ75" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="AK75" s="120" t="s">
+      <c r="AK75" s="119" t="s">
         <v>74</v>
       </c>
-      <c r="AL75" s="120" t="s">
+      <c r="AL75" s="119" t="s">
         <v>74</v>
       </c>
-      <c r="AM75" s="120" t="s">
+      <c r="AM75" s="119" t="s">
         <v>74</v>
       </c>
       <c r="AN75" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="AO75" s="120" t="s">
+      <c r="AO75" s="119" t="s">
         <v>74</v>
       </c>
-      <c r="AP75" s="120" t="s">
+      <c r="AP75" s="119" t="s">
         <v>74</v>
       </c>
       <c r="AQ75" s="51" t="s">
@@ -7325,7 +7286,7 @@
     </row>
     <row r="76" spans="1:69" s="17" customFormat="1" ht="15" thickTop="1">
       <c r="A76" s="45"/>
-      <c r="B76" s="69"/>
+      <c r="B76" s="123"/>
       <c r="C76" s="31"/>
       <c r="D76" s="45"/>
       <c r="E76" s="45"/>
@@ -7351,9 +7312,9 @@
       <c r="Y76" s="47"/>
       <c r="Z76" s="47"/>
       <c r="AA76" s="44"/>
-      <c r="AB76" s="123"/>
+      <c r="AB76" s="122"/>
       <c r="AC76" s="62"/>
-      <c r="AD76" s="127"/>
+      <c r="AD76" s="126"/>
       <c r="AE76" s="44"/>
       <c r="AF76" s="44"/>
       <c r="AG76"/>
@@ -15989,17 +15950,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="I73:N73"/>
-    <mergeCell ref="H63:M63"/>
-    <mergeCell ref="O73:T73"/>
-    <mergeCell ref="N63:S63"/>
-    <mergeCell ref="T63:T64"/>
     <mergeCell ref="AH73:AS73"/>
     <mergeCell ref="A73:H73"/>
     <mergeCell ref="W73:Z73"/>
     <mergeCell ref="D63:G63"/>
     <mergeCell ref="AA73:AG73"/>
     <mergeCell ref="A63:C63"/>
+    <mergeCell ref="I73:N73"/>
+    <mergeCell ref="H63:M63"/>
+    <mergeCell ref="O73:T73"/>
+    <mergeCell ref="N63:S63"/>
+    <mergeCell ref="T63:T64"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="11">

</xml_diff>